<commit_message>
Added Video and Made More Updates
Added the video and made more updates to the files. The assignment is no longer due today, so if things change I'll update this.
</commit_message>
<xml_diff>
--- a/roderick_montague_100701758_-_dgh-asn02_-_bill_materials.xlsx
+++ b/roderick_montague_100701758_-_dgh-asn02_-_bill_materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roder\Documents\University Materials\Year 4\Industrial Design for Game Hardware\DGH - ASN02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F4C83F-F663-4138-8B18-EEEE956E9407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE1D16D-6C9B-40CF-88B4-776388DBC27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11208" yWindow="0" windowWidth="11832" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Component</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>https://www.creatroninc.com/product/arduino-uno-rev3/</t>
+  </si>
+  <si>
+    <t>02/18/2022</t>
   </si>
 </sst>
 </file>
@@ -708,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,214 +742,219 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B9" s="15">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>14.75</v>
       </c>
-      <c r="D8" s="18">
-        <f>C8*B8</f>
+      <c r="D9" s="18">
+        <f>C9*B9</f>
         <v>73.75</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F9" s="21" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>27.99</v>
-      </c>
-      <c r="D9" s="18">
-        <f t="shared" ref="D9:D14" si="0">C9*B9</f>
-        <v>27.99</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>27.99</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" ref="D10:D15" si="0">C10*B10</f>
+        <v>27.99</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B11" s="15">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>3.59</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D11" s="18">
         <f t="shared" si="0"/>
         <v>17.95</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="15">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="D11" s="18">
-        <f>C11*2</f>
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="15">
+      <c r="C12" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="18">
+        <f>C12*2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="15">
         <v>1</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>1.5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D13" s="18">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B14" s="15">
         <f>13+2+21+21</f>
         <v>57</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <f>2.5</f>
         <v>2.5</v>
       </c>
-      <c r="D13" s="18">
-        <f>C13*6</f>
+      <c r="D14" s="18">
+        <f>C14*6</f>
         <v>15</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F14" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B15" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="10">
         <f>7.8</f>
         <v>7.8</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D15" s="19">
         <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F15" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="17">
-        <f>SUM(B8:B14)</f>
+      <c r="B16" s="17">
+        <f>SUM(B9:B15)</f>
         <v>81</v>
       </c>
-      <c r="C15" s="13">
-        <f>SUM(C8:C14)</f>
+      <c r="C16" s="13">
+        <f>SUM(C9:C15)</f>
         <v>58.379999999999995</v>
       </c>
-      <c r="D15" s="20">
-        <f>SUM(D8:D14)</f>
+      <c r="D16" s="20">
+        <f>SUM(D9:D15)</f>
         <v>144.49</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{337A5F60-75AF-46A0-9AC7-2C4F77720810}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{EFB6F78C-0A57-4541-8216-7AAB72B7AA8F}"/>
-    <hyperlink ref="F9" r:id="rId3" xr:uid="{5B5F5A51-9A67-4F82-9BEB-3E818727BC0F}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{1C1BD567-878F-4A3C-ABC7-8A20E8F9D36B}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{75CDD9B6-B93A-4AB9-9BE3-865E342FD05D}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{4818D00E-B8A2-4A52-BC93-297A366DD224}"/>
-    <hyperlink ref="F14" r:id="rId7" xr:uid="{8ACCF37A-2799-4A01-87F0-B085B5037CC5}"/>
-    <hyperlink ref="F13" r:id="rId8" xr:uid="{1673BF1E-BCE4-47ED-B021-23F654E90A0D}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{337A5F60-75AF-46A0-9AC7-2C4F77720810}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{EFB6F78C-0A57-4541-8216-7AAB72B7AA8F}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{5B5F5A51-9A67-4F82-9BEB-3E818727BC0F}"/>
+    <hyperlink ref="F12" r:id="rId4" xr:uid="{1C1BD567-878F-4A3C-ABC7-8A20E8F9D36B}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{75CDD9B6-B93A-4AB9-9BE3-865E342FD05D}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{4818D00E-B8A2-4A52-BC93-297A366DD224}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{8ACCF37A-2799-4A01-87F0-B085B5037CC5}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{1673BF1E-BCE4-47ED-B021-23F654E90A0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>

</xml_diff>